<commit_message>
update lines in experiments file
</commit_message>
<xml_diff>
--- a/Measurements.xlsx
+++ b/Measurements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7986B194-2091-49A9-85B7-829FE910D664}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9BF7C14-DBB6-4178-A85C-9CE5C60C827D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15465" windowHeight="7980" activeTab="1" xr2:uid="{BF278BFA-85CA-4AD2-B762-B86A01D98078}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{BF278BFA-85CA-4AD2-B762-B86A01D98078}"/>
   </bookViews>
   <sheets>
     <sheet name="Disks" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="32">
   <si>
     <t>d1</t>
   </si>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t>R75</t>
-  </si>
-  <si>
-    <t>R76</t>
   </si>
   <si>
     <t>R37</t>
@@ -2311,7 +2308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6589C76A-F353-4AF1-9FB2-7C280E2E3DA9}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14:D14"/>
     </sheetView>
   </sheetViews>
@@ -2521,7 +2518,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="12">
         <v>37600</v>
@@ -2535,7 +2532,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="12">
         <v>37600</v>
@@ -2549,7 +2546,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="12">
         <v>37600</v>
@@ -2563,7 +2560,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="12">
         <v>37500</v>
@@ -2577,7 +2574,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="12">
         <v>37500</v>
@@ -2591,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="12">
         <v>37600</v>
@@ -2605,7 +2602,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="12">
         <v>37500</v>
@@ -2619,7 +2616,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="12">
         <v>37500</v>
@@ -2633,7 +2630,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" s="12">
         <v>37600</v>
@@ -2647,7 +2644,7 @@
         <v>14</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="12">
         <v>37500</v>
@@ -2661,7 +2658,7 @@
         <v>15</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" s="12">
         <v>37400</v>
@@ -2675,7 +2672,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" s="12">
         <v>37800</v>
@@ -2689,7 +2686,7 @@
         <v>17</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" s="12">
         <v>37400</v>
@@ -2706,10 +2703,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DC2C71C-06BE-4D19-812B-BC6D8FE18F24}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2719,10 +2716,10 @@
         <v>18</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>19</v>
@@ -2745,7 +2742,7 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2762,7 +2759,7 @@
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2813,7 +2810,7 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2830,7 +2827,7 @@
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2847,7 +2844,1656 @@
         <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>180</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>260</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>260</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>260</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>260</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>180</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>180</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>180</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>180</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>260</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>260</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>260</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>260</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>180</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>180</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>180</v>
+      </c>
+      <c r="D24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>180</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>260</v>
+      </c>
+      <c r="D26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>260</v>
+      </c>
+      <c r="D27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>260</v>
+      </c>
+      <c r="D28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>260</v>
+      </c>
+      <c r="D29" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>180</v>
+      </c>
+      <c r="D30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>180</v>
+      </c>
+      <c r="D31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32">
+        <v>180</v>
+      </c>
+      <c r="D32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>180</v>
+      </c>
+      <c r="D33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>260</v>
+      </c>
+      <c r="D34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>260</v>
+      </c>
+      <c r="D35" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>260</v>
+      </c>
+      <c r="D36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>260</v>
+      </c>
+      <c r="D37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>180</v>
+      </c>
+      <c r="D38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <v>180</v>
+      </c>
+      <c r="D39" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40">
+        <v>6</v>
+      </c>
+      <c r="C40">
+        <v>180</v>
+      </c>
+      <c r="D40" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41">
+        <v>7</v>
+      </c>
+      <c r="C41">
+        <v>180</v>
+      </c>
+      <c r="D41" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>260</v>
+      </c>
+      <c r="D42" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>260</v>
+      </c>
+      <c r="D43" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <v>260</v>
+      </c>
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>260</v>
+      </c>
+      <c r="D45" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46">
+        <v>180</v>
+      </c>
+      <c r="D46" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47">
+        <v>180</v>
+      </c>
+      <c r="D47" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48">
+        <v>6</v>
+      </c>
+      <c r="C48">
+        <v>180</v>
+      </c>
+      <c r="D48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49">
+        <v>7</v>
+      </c>
+      <c r="C49">
+        <v>180</v>
+      </c>
+      <c r="D49" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>260</v>
+      </c>
+      <c r="D50" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>260</v>
+      </c>
+      <c r="D51" t="s">
+        <v>21</v>
+      </c>
+      <c r="E51" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>260</v>
+      </c>
+      <c r="D52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>260</v>
+      </c>
+      <c r="D53" t="s">
+        <v>21</v>
+      </c>
+      <c r="E53" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>180</v>
+      </c>
+      <c r="D54" t="s">
+        <v>20</v>
+      </c>
+      <c r="E54" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55">
+        <v>5</v>
+      </c>
+      <c r="C55">
+        <v>180</v>
+      </c>
+      <c r="D55" t="s">
+        <v>21</v>
+      </c>
+      <c r="E55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56">
+        <v>6</v>
+      </c>
+      <c r="C56">
+        <v>180</v>
+      </c>
+      <c r="D56" t="s">
+        <v>20</v>
+      </c>
+      <c r="E56" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57">
+        <v>7</v>
+      </c>
+      <c r="C57">
+        <v>180</v>
+      </c>
+      <c r="D57" t="s">
+        <v>21</v>
+      </c>
+      <c r="E57" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>260</v>
+      </c>
+      <c r="D58" t="s">
+        <v>20</v>
+      </c>
+      <c r="E58" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>260</v>
+      </c>
+      <c r="D59" t="s">
+        <v>21</v>
+      </c>
+      <c r="E59" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60">
+        <v>260</v>
+      </c>
+      <c r="D60" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61">
+        <v>3</v>
+      </c>
+      <c r="C61">
+        <v>260</v>
+      </c>
+      <c r="D61" t="s">
+        <v>21</v>
+      </c>
+      <c r="E61" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62">
+        <v>4</v>
+      </c>
+      <c r="C62">
+        <v>180</v>
+      </c>
+      <c r="D62" t="s">
+        <v>20</v>
+      </c>
+      <c r="E62" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63">
+        <v>5</v>
+      </c>
+      <c r="C63">
+        <v>180</v>
+      </c>
+      <c r="D63" t="s">
+        <v>21</v>
+      </c>
+      <c r="E63" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64">
+        <v>6</v>
+      </c>
+      <c r="C64">
+        <v>180</v>
+      </c>
+      <c r="D64" t="s">
+        <v>20</v>
+      </c>
+      <c r="E64" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65">
+        <v>7</v>
+      </c>
+      <c r="C65">
+        <v>180</v>
+      </c>
+      <c r="D65" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>260</v>
+      </c>
+      <c r="D66" t="s">
+        <v>20</v>
+      </c>
+      <c r="E66" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>13</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>260</v>
+      </c>
+      <c r="D67" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>13</v>
+      </c>
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68">
+        <v>260</v>
+      </c>
+      <c r="D68" t="s">
+        <v>20</v>
+      </c>
+      <c r="E68" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69">
+        <v>3</v>
+      </c>
+      <c r="C69">
+        <v>260</v>
+      </c>
+      <c r="D69" t="s">
+        <v>21</v>
+      </c>
+      <c r="E69" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>13</v>
+      </c>
+      <c r="B70">
+        <v>4</v>
+      </c>
+      <c r="C70">
+        <v>180</v>
+      </c>
+      <c r="D70" t="s">
+        <v>20</v>
+      </c>
+      <c r="E70" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71">
+        <v>5</v>
+      </c>
+      <c r="C71">
+        <v>180</v>
+      </c>
+      <c r="D71" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>13</v>
+      </c>
+      <c r="B72">
+        <v>6</v>
+      </c>
+      <c r="C72">
+        <v>180</v>
+      </c>
+      <c r="D72" t="s">
+        <v>20</v>
+      </c>
+      <c r="E72" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>13</v>
+      </c>
+      <c r="B73">
+        <v>7</v>
+      </c>
+      <c r="C73">
+        <v>180</v>
+      </c>
+      <c r="D73" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>14</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>260</v>
+      </c>
+      <c r="D74" t="s">
+        <v>20</v>
+      </c>
+      <c r="E74" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>14</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <v>260</v>
+      </c>
+      <c r="D75" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>14</v>
+      </c>
+      <c r="B76">
+        <v>2</v>
+      </c>
+      <c r="C76">
+        <v>260</v>
+      </c>
+      <c r="D76" t="s">
+        <v>20</v>
+      </c>
+      <c r="E76" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77">
+        <v>3</v>
+      </c>
+      <c r="C77">
+        <v>260</v>
+      </c>
+      <c r="D77" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78">
+        <v>4</v>
+      </c>
+      <c r="C78">
+        <v>180</v>
+      </c>
+      <c r="D78" t="s">
+        <v>20</v>
+      </c>
+      <c r="E78" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>14</v>
+      </c>
+      <c r="B79">
+        <v>5</v>
+      </c>
+      <c r="C79">
+        <v>180</v>
+      </c>
+      <c r="D79" t="s">
+        <v>21</v>
+      </c>
+      <c r="E79" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>14</v>
+      </c>
+      <c r="B80">
+        <v>6</v>
+      </c>
+      <c r="C80">
+        <v>180</v>
+      </c>
+      <c r="D80" t="s">
+        <v>20</v>
+      </c>
+      <c r="E80" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>14</v>
+      </c>
+      <c r="B81">
+        <v>7</v>
+      </c>
+      <c r="C81">
+        <v>180</v>
+      </c>
+      <c r="D81" t="s">
+        <v>21</v>
+      </c>
+      <c r="E81" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>15</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>260</v>
+      </c>
+      <c r="D82" t="s">
+        <v>20</v>
+      </c>
+      <c r="E82" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>15</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83">
+        <v>260</v>
+      </c>
+      <c r="D83" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>15</v>
+      </c>
+      <c r="B84">
+        <v>2</v>
+      </c>
+      <c r="C84">
+        <v>260</v>
+      </c>
+      <c r="D84" t="s">
+        <v>20</v>
+      </c>
+      <c r="E84" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>15</v>
+      </c>
+      <c r="B85">
+        <v>3</v>
+      </c>
+      <c r="C85">
+        <v>260</v>
+      </c>
+      <c r="D85" t="s">
+        <v>21</v>
+      </c>
+      <c r="E85" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>15</v>
+      </c>
+      <c r="B86">
+        <v>4</v>
+      </c>
+      <c r="C86">
+        <v>180</v>
+      </c>
+      <c r="D86" t="s">
+        <v>20</v>
+      </c>
+      <c r="E86" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>15</v>
+      </c>
+      <c r="B87">
+        <v>5</v>
+      </c>
+      <c r="C87">
+        <v>180</v>
+      </c>
+      <c r="D87" t="s">
+        <v>21</v>
+      </c>
+      <c r="E87" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>15</v>
+      </c>
+      <c r="B88">
+        <v>6</v>
+      </c>
+      <c r="C88">
+        <v>180</v>
+      </c>
+      <c r="D88" t="s">
+        <v>20</v>
+      </c>
+      <c r="E88" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>15</v>
+      </c>
+      <c r="B89">
+        <v>7</v>
+      </c>
+      <c r="C89">
+        <v>180</v>
+      </c>
+      <c r="D89" t="s">
+        <v>21</v>
+      </c>
+      <c r="E89" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>16</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>260</v>
+      </c>
+      <c r="D90" t="s">
+        <v>20</v>
+      </c>
+      <c r="E90" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>16</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91">
+        <v>260</v>
+      </c>
+      <c r="D91" t="s">
+        <v>21</v>
+      </c>
+      <c r="E91" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>16</v>
+      </c>
+      <c r="B92">
+        <v>2</v>
+      </c>
+      <c r="C92">
+        <v>260</v>
+      </c>
+      <c r="D92" t="s">
+        <v>20</v>
+      </c>
+      <c r="E92" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>16</v>
+      </c>
+      <c r="B93">
+        <v>3</v>
+      </c>
+      <c r="C93">
+        <v>260</v>
+      </c>
+      <c r="D93" t="s">
+        <v>21</v>
+      </c>
+      <c r="E93" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>16</v>
+      </c>
+      <c r="B94">
+        <v>4</v>
+      </c>
+      <c r="C94">
+        <v>180</v>
+      </c>
+      <c r="D94" t="s">
+        <v>20</v>
+      </c>
+      <c r="E94" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>16</v>
+      </c>
+      <c r="B95">
+        <v>5</v>
+      </c>
+      <c r="C95">
+        <v>180</v>
+      </c>
+      <c r="D95" t="s">
+        <v>21</v>
+      </c>
+      <c r="E95" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>16</v>
+      </c>
+      <c r="B96">
+        <v>6</v>
+      </c>
+      <c r="C96">
+        <v>180</v>
+      </c>
+      <c r="D96" t="s">
+        <v>20</v>
+      </c>
+      <c r="E96" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>16</v>
+      </c>
+      <c r="B97">
+        <v>7</v>
+      </c>
+      <c r="C97">
+        <v>180</v>
+      </c>
+      <c r="D97" t="s">
+        <v>21</v>
+      </c>
+      <c r="E97" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>17</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>260</v>
+      </c>
+      <c r="D98" t="s">
+        <v>20</v>
+      </c>
+      <c r="E98" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>17</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="C99">
+        <v>260</v>
+      </c>
+      <c r="D99" t="s">
+        <v>21</v>
+      </c>
+      <c r="E99" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>17</v>
+      </c>
+      <c r="B100">
+        <v>2</v>
+      </c>
+      <c r="C100">
+        <v>260</v>
+      </c>
+      <c r="D100" t="s">
+        <v>20</v>
+      </c>
+      <c r="E100" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>17</v>
+      </c>
+      <c r="B101">
+        <v>3</v>
+      </c>
+      <c r="C101">
+        <v>260</v>
+      </c>
+      <c r="D101" t="s">
+        <v>21</v>
+      </c>
+      <c r="E101" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>17</v>
+      </c>
+      <c r="B102">
+        <v>4</v>
+      </c>
+      <c r="C102">
+        <v>180</v>
+      </c>
+      <c r="D102" t="s">
+        <v>20</v>
+      </c>
+      <c r="E102" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>17</v>
+      </c>
+      <c r="B103">
+        <v>5</v>
+      </c>
+      <c r="C103">
+        <v>180</v>
+      </c>
+      <c r="D103" t="s">
+        <v>21</v>
+      </c>
+      <c r="E103" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>17</v>
+      </c>
+      <c r="B104">
+        <v>6</v>
+      </c>
+      <c r="C104">
+        <v>180</v>
+      </c>
+      <c r="D104" t="s">
+        <v>20</v>
+      </c>
+      <c r="E104" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>17</v>
+      </c>
+      <c r="B105">
+        <v>7</v>
+      </c>
+      <c r="C105">
+        <v>180</v>
+      </c>
+      <c r="D105" t="s">
+        <v>21</v>
+      </c>
+      <c r="E105" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>